<commit_message>
Stephan is done :)
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19109"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E7DE755-77FE-44F1-AEB6-324BFA3F75BE}" xr6:coauthVersionLast="29" xr6:coauthVersionMax="29" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="12" windowWidth="19068" windowHeight="8676"/>
+    <workbookView xWindow="120" yWindow="12" windowWidth="19068" windowHeight="8676" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="111" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179016"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
   <si>
+    <t>Oleg</t>
+  </si>
+  <si>
     <t>56 - 66</t>
   </si>
   <si>
@@ -331,6 +335,12 @@
     <t>4687 - 4697</t>
   </si>
   <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>1-11</t>
+  </si>
+  <si>
     <t>78 - 88</t>
   </si>
   <si>
@@ -682,6 +692,12 @@
     <t>4731 - 4732</t>
   </si>
   <si>
+    <t>Stephan</t>
+  </si>
+  <si>
+    <t>12-22</t>
+  </si>
+  <si>
     <t>23 - 33</t>
   </si>
   <si>
@@ -997,6 +1013,9 @@
     <t>4720 - 4730</t>
   </si>
   <si>
+    <t>4th</t>
+  </si>
+  <si>
     <t>34 - 44</t>
   </si>
   <si>
@@ -1301,31 +1320,13 @@
   </si>
   <si>
     <t>4709 - 4719</t>
-  </si>
-  <si>
-    <t>1-11</t>
-  </si>
-  <si>
-    <t>12-22</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
-    <t>3rd</t>
-  </si>
-  <si>
-    <t>4th</t>
-  </si>
-  <si>
-    <t>Oleg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1826,48 +1827,48 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1875,14 +1876,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1920,9 +1924,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1955,9 +1959,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1990,9 +2011,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2165,1326 +2203,1326 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:119" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:119">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:119">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P2" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>122</v>
+      </c>
+      <c r="R2" t="s">
+        <v>123</v>
+      </c>
+      <c r="S2" t="s">
+        <v>124</v>
+      </c>
+      <c r="T2" t="s">
+        <v>125</v>
+      </c>
+      <c r="U2" t="s">
+        <v>126</v>
+      </c>
+      <c r="V2" t="s">
+        <v>127</v>
+      </c>
+      <c r="W2" t="s">
+        <v>128</v>
+      </c>
+      <c r="X2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>157</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>158</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>159</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>160</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>161</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>164</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>166</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>167</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>170</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>172</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>173</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>174</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>175</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>176</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>177</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>178</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>179</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>181</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>182</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>183</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>184</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>185</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>186</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>187</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>188</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>189</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>190</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>191</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>192</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>193</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>194</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>195</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>196</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>197</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>198</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>199</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>200</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>201</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>202</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>204</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>205</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>206</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>207</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>208</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>209</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>210</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>211</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>212</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>213</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>214</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>215</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>216</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>217</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>218</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>219</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>220</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>221</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>222</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>223</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:119">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H3" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" t="s">
+        <v>233</v>
+      </c>
+      <c r="J3" t="s">
+        <v>234</v>
+      </c>
+      <c r="K3" t="s">
+        <v>235</v>
+      </c>
+      <c r="L3" t="s">
+        <v>236</v>
+      </c>
+      <c r="M3" t="s">
+        <v>237</v>
+      </c>
+      <c r="N3" t="s">
+        <v>238</v>
+      </c>
+      <c r="O3" t="s">
+        <v>239</v>
+      </c>
+      <c r="P3" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>241</v>
+      </c>
+      <c r="R3" t="s">
+        <v>242</v>
+      </c>
+      <c r="S3" t="s">
+        <v>243</v>
+      </c>
+      <c r="T3" t="s">
+        <v>244</v>
+      </c>
+      <c r="U3" t="s">
+        <v>245</v>
+      </c>
+      <c r="V3" t="s">
+        <v>246</v>
+      </c>
+      <c r="W3" t="s">
+        <v>247</v>
+      </c>
+      <c r="X3" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>252</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>254</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>255</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>258</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>260</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>261</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>262</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>263</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>264</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>265</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>266</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>267</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>268</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>269</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>270</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>273</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>274</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>275</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>277</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>278</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>279</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>280</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>281</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>283</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>284</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>285</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>287</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>288</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>289</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>290</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>291</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>292</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>295</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>296</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>297</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>298</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>299</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>301</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>302</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>303</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>304</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>305</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>306</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>307</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>308</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>309</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>310</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>311</v>
+      </c>
+      <c r="CJ3" t="s">
+        <v>312</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>313</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>314</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>315</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>316</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>317</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>318</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>319</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>320</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>321</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>322</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>323</v>
+      </c>
+      <c r="CV3" t="s">
+        <v>324</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>325</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>326</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>327</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>328</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>329</v>
+      </c>
+      <c r="DB3" t="s">
+        <v>330</v>
+      </c>
+      <c r="DC3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:119">
+      <c r="A4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F4" t="s">
+        <v>337</v>
+      </c>
+      <c r="G4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H4" t="s">
+        <v>339</v>
+      </c>
+      <c r="I4" t="s">
+        <v>340</v>
+      </c>
+      <c r="J4" t="s">
+        <v>341</v>
+      </c>
+      <c r="K4" t="s">
+        <v>342</v>
+      </c>
+      <c r="L4" t="s">
+        <v>343</v>
+      </c>
+      <c r="M4" t="s">
+        <v>344</v>
+      </c>
+      <c r="N4" t="s">
+        <v>345</v>
+      </c>
+      <c r="O4" t="s">
+        <v>346</v>
+      </c>
+      <c r="P4" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>348</v>
+      </c>
+      <c r="R4" t="s">
+        <v>349</v>
+      </c>
+      <c r="S4" t="s">
+        <v>350</v>
+      </c>
+      <c r="T4" t="s">
+        <v>351</v>
+      </c>
+      <c r="U4" t="s">
+        <v>352</v>
+      </c>
+      <c r="V4" t="s">
+        <v>353</v>
+      </c>
+      <c r="W4" t="s">
+        <v>354</v>
+      </c>
+      <c r="X4" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>356</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>357</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>361</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>362</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>363</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>364</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>365</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>366</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>367</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>368</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>369</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>370</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>371</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>372</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>373</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>374</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>375</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>376</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>377</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>378</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>379</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>380</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>381</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>382</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>383</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>384</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>385</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>386</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>387</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>388</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>389</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>390</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>391</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>392</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>394</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>395</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>396</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>397</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>398</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>399</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>400</v>
+      </c>
+      <c r="BR4" t="s">
+        <v>401</v>
+      </c>
+      <c r="BS4" t="s">
+        <v>402</v>
+      </c>
+      <c r="BT4" t="s">
+        <v>403</v>
+      </c>
+      <c r="BU4" t="s">
+        <v>404</v>
+      </c>
+      <c r="BV4" t="s">
+        <v>405</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>406</v>
+      </c>
+      <c r="BX4" t="s">
+        <v>407</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>408</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>409</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>410</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>411</v>
+      </c>
+      <c r="CC4" t="s">
+        <v>412</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>413</v>
+      </c>
+      <c r="CE4" t="s">
+        <v>414</v>
+      </c>
+      <c r="CF4" t="s">
+        <v>415</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>416</v>
+      </c>
+      <c r="CH4" t="s">
+        <v>417</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>418</v>
+      </c>
+      <c r="CJ4" t="s">
+        <v>419</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>420</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>421</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>422</v>
+      </c>
+      <c r="CN4" t="s">
+        <v>423</v>
+      </c>
+      <c r="CO4" t="s">
+        <v>424</v>
+      </c>
+      <c r="CP4" t="s">
+        <v>425</v>
+      </c>
+      <c r="CQ4" t="s">
+        <v>426</v>
+      </c>
+      <c r="CR4" t="s">
+        <v>427</v>
+      </c>
+      <c r="CS4" t="s">
+        <v>428</v>
+      </c>
+      <c r="CT4" t="s">
+        <v>429</v>
+      </c>
+      <c r="CU4" t="s">
+        <v>430</v>
+      </c>
+      <c r="CV4" t="s">
+        <v>431</v>
+      </c>
+      <c r="CW4" t="s">
+        <v>432</v>
+      </c>
+      <c r="CX4" t="s">
+        <v>433</v>
+      </c>
+      <c r="CY4" t="s">
         <v>434</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>76</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>81</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>83</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>85</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>86</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>90</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>91</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>92</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>93</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>94</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>95</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>96</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>100</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>101</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>102</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>103</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:119" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>431</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" t="s">
-        <v>111</v>
-      </c>
-      <c r="J2" t="s">
-        <v>112</v>
-      </c>
-      <c r="K2" t="s">
-        <v>113</v>
-      </c>
-      <c r="L2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M2" t="s">
-        <v>115</v>
-      </c>
-      <c r="N2" t="s">
-        <v>116</v>
-      </c>
-      <c r="O2" t="s">
-        <v>117</v>
-      </c>
-      <c r="P2" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" t="s">
-        <v>120</v>
-      </c>
-      <c r="S2" t="s">
-        <v>121</v>
-      </c>
-      <c r="T2" t="s">
-        <v>122</v>
-      </c>
-      <c r="U2" t="s">
-        <v>123</v>
-      </c>
-      <c r="V2" t="s">
-        <v>124</v>
-      </c>
-      <c r="W2" t="s">
-        <v>125</v>
-      </c>
-      <c r="X2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>155</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>156</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>157</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>158</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>159</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>160</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>161</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>162</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>163</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>164</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>165</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>166</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>167</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>168</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>169</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>170</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>171</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>172</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>173</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>174</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>175</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>176</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>177</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>178</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>179</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>180</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>182</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>183</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>184</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>185</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>186</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>187</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>188</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>189</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>190</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>191</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>192</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>193</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>194</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>195</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>196</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>197</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>198</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>199</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>200</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>201</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>202</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>204</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>205</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>206</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>207</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>208</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>209</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>210</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>211</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>212</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>214</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>216</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>217</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>218</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>219</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>220</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:119" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>432</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E3" t="s">
-        <v>224</v>
-      </c>
-      <c r="F3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G3" t="s">
-        <v>226</v>
-      </c>
-      <c r="H3" t="s">
-        <v>227</v>
-      </c>
-      <c r="I3" t="s">
-        <v>228</v>
-      </c>
-      <c r="J3" t="s">
-        <v>229</v>
-      </c>
-      <c r="K3" t="s">
-        <v>230</v>
-      </c>
-      <c r="L3" t="s">
-        <v>231</v>
-      </c>
-      <c r="M3" t="s">
-        <v>232</v>
-      </c>
-      <c r="N3" t="s">
-        <v>233</v>
-      </c>
-      <c r="O3" t="s">
-        <v>234</v>
-      </c>
-      <c r="P3" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>236</v>
-      </c>
-      <c r="R3" t="s">
-        <v>237</v>
-      </c>
-      <c r="S3" t="s">
-        <v>238</v>
-      </c>
-      <c r="T3" t="s">
-        <v>239</v>
-      </c>
-      <c r="U3" t="s">
-        <v>240</v>
-      </c>
-      <c r="V3" t="s">
-        <v>241</v>
-      </c>
-      <c r="W3" t="s">
-        <v>242</v>
-      </c>
-      <c r="X3" t="s">
-        <v>243</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>245</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>246</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>247</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>248</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>249</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>250</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>251</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>252</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>253</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>254</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>255</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>256</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>257</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>258</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>259</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>260</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>261</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>262</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>263</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>264</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>265</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>266</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>267</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>268</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>269</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>270</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>271</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>272</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>273</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>274</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>275</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>276</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>277</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>278</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>279</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>280</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>281</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>282</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>283</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>284</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>285</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>286</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>287</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>288</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>289</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>290</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>291</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>292</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>293</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>294</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>295</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>296</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>297</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>298</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>299</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>300</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>301</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>302</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>303</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>304</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>305</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>306</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>307</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>308</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>309</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>310</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>311</v>
-      </c>
-      <c r="CO3" t="s">
-        <v>312</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>313</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>314</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>315</v>
-      </c>
-      <c r="CS3" t="s">
-        <v>316</v>
-      </c>
-      <c r="CT3" t="s">
-        <v>317</v>
-      </c>
-      <c r="CU3" t="s">
-        <v>318</v>
-      </c>
-      <c r="CV3" t="s">
-        <v>319</v>
-      </c>
-      <c r="CW3" t="s">
-        <v>320</v>
-      </c>
-      <c r="CX3" t="s">
-        <v>321</v>
-      </c>
-      <c r="CY3" t="s">
-        <v>322</v>
-      </c>
-      <c r="CZ3" t="s">
-        <v>323</v>
-      </c>
-      <c r="DA3" t="s">
-        <v>324</v>
-      </c>
-      <c r="DB3" t="s">
-        <v>325</v>
-      </c>
-      <c r="DC3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="4" spans="1:119" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>433</v>
-      </c>
-      <c r="B4" t="s">
-        <v>327</v>
-      </c>
-      <c r="C4" t="s">
-        <v>328</v>
-      </c>
-      <c r="D4" t="s">
-        <v>329</v>
-      </c>
-      <c r="E4" t="s">
-        <v>330</v>
-      </c>
-      <c r="F4" t="s">
-        <v>331</v>
-      </c>
-      <c r="G4" t="s">
-        <v>332</v>
-      </c>
-      <c r="H4" t="s">
-        <v>333</v>
-      </c>
-      <c r="I4" t="s">
-        <v>334</v>
-      </c>
-      <c r="J4" t="s">
-        <v>335</v>
-      </c>
-      <c r="K4" t="s">
-        <v>336</v>
-      </c>
-      <c r="L4" t="s">
-        <v>337</v>
-      </c>
-      <c r="M4" t="s">
-        <v>338</v>
-      </c>
-      <c r="N4" t="s">
-        <v>339</v>
-      </c>
-      <c r="O4" t="s">
-        <v>340</v>
-      </c>
-      <c r="P4" t="s">
-        <v>341</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>342</v>
-      </c>
-      <c r="R4" t="s">
-        <v>343</v>
-      </c>
-      <c r="S4" t="s">
-        <v>344</v>
-      </c>
-      <c r="T4" t="s">
-        <v>345</v>
-      </c>
-      <c r="U4" t="s">
-        <v>346</v>
-      </c>
-      <c r="V4" t="s">
-        <v>347</v>
-      </c>
-      <c r="W4" t="s">
-        <v>348</v>
-      </c>
-      <c r="X4" t="s">
-        <v>349</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>350</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>351</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>352</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>354</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>355</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>356</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>357</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>358</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>359</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>360</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>361</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>362</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>363</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>364</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>365</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>366</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>367</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>368</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>369</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>370</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>371</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>372</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>373</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>374</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>375</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>376</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>377</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>378</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>379</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>380</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>381</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>382</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>383</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>384</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>385</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>386</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>387</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>388</v>
-      </c>
-      <c r="BL4" t="s">
-        <v>389</v>
-      </c>
-      <c r="BM4" t="s">
-        <v>390</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>391</v>
-      </c>
-      <c r="BO4" t="s">
-        <v>392</v>
-      </c>
-      <c r="BP4" t="s">
-        <v>393</v>
-      </c>
-      <c r="BQ4" t="s">
-        <v>394</v>
-      </c>
-      <c r="BR4" t="s">
-        <v>395</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>396</v>
-      </c>
-      <c r="BT4" t="s">
-        <v>397</v>
-      </c>
-      <c r="BU4" t="s">
-        <v>398</v>
-      </c>
-      <c r="BV4" t="s">
-        <v>399</v>
-      </c>
-      <c r="BW4" t="s">
-        <v>400</v>
-      </c>
-      <c r="BX4" t="s">
-        <v>401</v>
-      </c>
-      <c r="BY4" t="s">
-        <v>402</v>
-      </c>
-      <c r="BZ4" t="s">
-        <v>403</v>
-      </c>
-      <c r="CA4" t="s">
-        <v>404</v>
-      </c>
-      <c r="CB4" t="s">
-        <v>405</v>
-      </c>
-      <c r="CC4" t="s">
-        <v>406</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>407</v>
-      </c>
-      <c r="CE4" t="s">
-        <v>408</v>
-      </c>
-      <c r="CF4" t="s">
-        <v>409</v>
-      </c>
-      <c r="CG4" t="s">
-        <v>410</v>
-      </c>
-      <c r="CH4" t="s">
-        <v>411</v>
-      </c>
-      <c r="CI4" t="s">
-        <v>412</v>
-      </c>
-      <c r="CJ4" t="s">
-        <v>413</v>
-      </c>
-      <c r="CK4" t="s">
-        <v>414</v>
-      </c>
-      <c r="CL4" t="s">
-        <v>415</v>
-      </c>
-      <c r="CM4" t="s">
-        <v>416</v>
-      </c>
-      <c r="CN4" t="s">
-        <v>417</v>
-      </c>
-      <c r="CO4" t="s">
-        <v>418</v>
-      </c>
-      <c r="CP4" t="s">
-        <v>419</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>420</v>
-      </c>
-      <c r="CR4" t="s">
-        <v>421</v>
-      </c>
-      <c r="CS4" t="s">
-        <v>422</v>
-      </c>
-      <c r="CT4" t="s">
-        <v>423</v>
-      </c>
-      <c r="CU4" t="s">
-        <v>424</v>
-      </c>
-      <c r="CV4" t="s">
-        <v>425</v>
-      </c>
-      <c r="CW4" t="s">
-        <v>426</v>
-      </c>
-      <c r="CX4" t="s">
-        <v>427</v>
-      </c>
-      <c r="CY4" t="s">
-        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>